<commit_message>
New improvements on the UI
</commit_message>
<xml_diff>
--- a/Backend/ANSC121.xlsx
+++ b/Backend/ANSC121.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dereck.ibale\Desktop\Proj A\Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{166122F0-4136-4D9E-8B72-48FBA5CF4D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860B1B08-C114-4502-8F1B-B308CAEF7060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>21-1-00346</t>
   </si>
@@ -210,6 +210,18 @@
   </si>
   <si>
     <t>biyatch</t>
+  </si>
+  <si>
+    <t>What is the date today?</t>
+  </si>
+  <si>
+    <t>Jan. 11, 2023</t>
+  </si>
+  <si>
+    <t>Feb. 2, 2024</t>
+  </si>
+  <si>
+    <t>Sep. 06, 1921</t>
   </si>
 </sst>
 </file>
@@ -247,7 +259,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -257,12 +269,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -282,7 +288,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -303,7 +309,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2563,10 +2570,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C92CBA4A-2255-477D-9260-14F38580C045}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2635,7 +2642,7 @@
       <c r="E3">
         <v>8</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="10">
         <v>10</v>
       </c>
     </row>
@@ -2675,7 +2682,7 @@
       <c r="E5">
         <v>11</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="10">
         <v>29</v>
       </c>
     </row>
@@ -2695,8 +2702,28 @@
       <c r="E6" t="s">
         <v>59</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="10" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="11">
+        <v>35860</v>
+      </c>
+      <c r="E7" s="11">
+        <v>38785</v>
+      </c>
+      <c r="F7" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I was able to extract the correct answers on backend side and added new component on frontend side
</commit_message>
<xml_diff>
--- a/Backend/ANSC121.xlsx
+++ b/Backend/ANSC121.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dereck.ibale\Desktop\Proj A\Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860B1B08-C114-4502-8F1B-B308CAEF7060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689636DD-3ACF-4FAE-A0F9-9D6F3DDEE3C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9170" yWindow="690" windowWidth="9260" windowHeight="9460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t>21-1-00346</t>
   </si>
@@ -188,40 +188,94 @@
     <t>What is 24 + 23</t>
   </si>
   <si>
-    <t>What are the complete names of this platform's creator</t>
-  </si>
-  <si>
-    <t>I don't know</t>
-  </si>
-  <si>
-    <t>biyatches</t>
-  </si>
-  <si>
-    <t>idc</t>
-  </si>
-  <si>
-    <t>taga bukid</t>
-  </si>
-  <si>
-    <t>maybe</t>
-  </si>
-  <si>
     <t>15-1-02342</t>
   </si>
   <si>
     <t>biyatch</t>
   </si>
   <si>
-    <t>What is the date today?</t>
-  </si>
-  <si>
     <t>Jan. 11, 2023</t>
   </si>
   <si>
-    <t>Feb. 2, 2024</t>
-  </si>
-  <si>
     <t>Sep. 06, 1921</t>
+  </si>
+  <si>
+    <t>It is called the river of life</t>
+  </si>
+  <si>
+    <t>Nile River</t>
+  </si>
+  <si>
+    <t>Blood</t>
+  </si>
+  <si>
+    <t>Pasig River</t>
+  </si>
+  <si>
+    <t>Rivermaya</t>
+  </si>
+  <si>
+    <t>Egyptian River</t>
+  </si>
+  <si>
+    <t>When is the World War I</t>
+  </si>
+  <si>
+    <t>Dec. 11, 1998</t>
+  </si>
+  <si>
+    <t>What is the chemical symbol for element Gold?</t>
+  </si>
+  <si>
+    <t>Au</t>
+  </si>
+  <si>
+    <t>Ag</t>
+  </si>
+  <si>
+    <t>Fe</t>
+  </si>
+  <si>
+    <t>Hg</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>What is the capital of France?</t>
+  </si>
+  <si>
+    <t>Madrid</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>Rome</t>
+  </si>
+  <si>
+    <t>Manila</t>
+  </si>
+  <si>
+    <t>What is the powerhouse of the cell?</t>
+  </si>
+  <si>
+    <t>Nucleus</t>
+  </si>
+  <si>
+    <t>Mitochondria</t>
+  </si>
+  <si>
+    <t>Endoplasmic Reticulum</t>
+  </si>
+  <si>
+    <t>Golgi Apparatus</t>
+  </si>
+  <si>
+    <t>None of the Above</t>
   </si>
 </sst>
 </file>
@@ -288,7 +342,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -311,6 +365,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1634,10 +1689,10 @@
     </row>
     <row r="24" spans="1:36" ht="21.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A24" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -2570,10 +2625,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C92CBA4A-2255-477D-9260-14F38580C045}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2688,42 +2743,102 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="11">
-        <v>35860</v>
+        <v>57</v>
+      </c>
+      <c r="C7" s="12">
+        <v>5323</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="E7" s="11">
         <v>38785</v>
       </c>
       <c r="F7" t="s">
-        <v>66</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I can render the score in the webpage
</commit_message>
<xml_diff>
--- a/Backend/ANSC121.xlsx
+++ b/Backend/ANSC121.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dereck.ibale\Desktop\Proj A\Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689636DD-3ACF-4FAE-A0F9-9D6F3DDEE3C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8888CC-5EA6-43BF-BBC0-733BB5E932F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9170" yWindow="690" windowWidth="9260" windowHeight="9460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t>21-1-00346</t>
   </si>
@@ -276,6 +276,9 @@
   </si>
   <si>
     <t>None of the Above</t>
+  </si>
+  <si>
+    <t>Jul. 28, 1914</t>
   </si>
 </sst>
 </file>
@@ -2627,8 +2630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C92CBA4A-2255-477D-9260-14F38580C045}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2768,8 +2771,8 @@
       <c r="B7" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="12">
-        <v>5323</v>
+      <c r="C7" s="12" t="s">
+        <v>85</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>66</v>

</xml_diff>